<commit_message>
mejoras para subir archivos
</commit_message>
<xml_diff>
--- a/public/tmp/prueba.xlsx
+++ b/public/tmp/prueba.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Nombre</t>
   </si>
@@ -147,6 +147,15 @@
   </si>
   <si>
     <t>jparbros@hotmail.com</t>
+  </si>
+  <si>
+    <t>Organizacion</t>
+  </si>
+  <si>
+    <t>ParBros</t>
+  </si>
+  <si>
+    <t>centro</t>
   </si>
 </sst>
 </file>
@@ -586,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -597,7 +606,7 @@
     <col min="25" max="25" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="36">
+    <row r="1" spans="1:26" ht="36">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -673,8 +682,11 @@
       <c r="Y1" s="5" t="s">
         <v>38</v>
       </c>
+      <c r="Z1" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" ht="36">
+    <row r="2" spans="1:26" ht="36">
       <c r="A2" s="4" t="s">
         <v>24</v>
       </c>
@@ -690,8 +702,8 @@
       <c r="E2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="1">
-        <v>3</v>
+      <c r="F2" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>28</v>
@@ -745,6 +757,9 @@
       <c r="X2" s="1"/>
       <c r="Y2">
         <v>3121385300</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>